<commit_message>
Deploying to gh-pages from  @ f370223bb5ef05ff408a430c361d43eaedd51c66 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.5.1.xlsx
+++ b/en/downloads/data-excel/1.5.1.xlsx
@@ -8167,7 +8167,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8746,7 +8746,7 @@
         <v>48</v>
       </c>
       <c r="Q13" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>